<commit_message>
added signup signin pages, added db, updated homepage.....Issues: signin and signup cause errors, insufficient css and more......needs working navbar
</commit_message>
<xml_diff>
--- a/hotel-booking-backend/server/hotel-database.xlsx
+++ b/hotel-booking-backend/server/hotel-database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HotelBookingApp\hotel-booking-backend\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HotelBookingGithubRepo\hotel-booking-backend\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95F8D00-D1F3-48B9-9BA4-2F80AB79EFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2744EF-7C1B-4F1E-8897-C9619C6D3B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E499A8B5-429D-4419-BB98-7D9C2D739F56}"/>
   </bookViews>
@@ -1310,7 +1310,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G1" sqref="G1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1497,5 +1497,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>